<commit_message>
move unit header to left and hide dashboard menu
</commit_message>
<xml_diff>
--- a/Activity Report.xlsx
+++ b/Activity Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devels\upskill\++\Skripsi-SistemPrediksi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B96C774-03FF-4EA8-9B4C-6DA193C7D97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9919B3-D5E8-481F-A030-9263D7FDD340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2140" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{DCD5F5CA-E4BE-4448-B88C-BBF8CC34712D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{DCD5F5CA-E4BE-4448-B88C-BBF8CC34712D}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Request" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Tanggal</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>Project documentation</t>
+  </si>
+  <si>
+    <t>Move unit header to the left, hide dashboard menu</t>
+  </si>
+  <si>
+    <t>paid</t>
+  </si>
+  <si>
+    <t>remaining</t>
   </si>
 </sst>
 </file>
@@ -613,10 +622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A270A0-1C0D-4975-BC77-8041C533A9AE}">
-  <dimension ref="A2:D18"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,21 +634,29 @@
     <col min="2" max="2" width="54.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="5">
         <f>SUM(Table2[Durasi (menit)])/60</f>
-        <v>14.25</v>
+        <v>14.5</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <f>7.125</f>
+        <v>7.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -649,8 +666,15 @@
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <f>C2-F2</f>
+        <v>7.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44909</v>
       </c>
@@ -661,7 +685,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -669,7 +693,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -677,7 +701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -685,7 +709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -693,7 +717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44910</v>
       </c>
@@ -704,7 +728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -712,7 +736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44911</v>
       </c>
@@ -723,7 +747,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44912</v>
       </c>
@@ -734,7 +758,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -742,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -750,7 +774,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44913</v>
       </c>
@@ -761,7 +785,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -786,6 +810,17 @@
       </c>
       <c r="C18" s="5">
         <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>44941</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>